<commit_message>
Update PI logic: Handle discounts and add surcharge table
</commit_message>
<xml_diff>
--- a/templates/proforma_invoice_template_no_discount.xlsx
+++ b/templates/proforma_invoice_template_no_discount.xlsx
@@ -65,7 +65,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -135,11 +135,18 @@
       <bottom style="thin"/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -159,9 +166,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -540,7 +549,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N34"/>
+  <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -745,76 +754,60 @@
           <t>{{Contract__c.Export_Route_Carrier__c}}</t>
         </is>
       </c>
-      <c r="D10" s="5" t="n"/>
-      <c r="E10" s="5" t="n"/>
-      <c r="F10" s="4" t="n"/>
-      <c r="G10" s="6" t="inlineStr">
-        <is>
-          <t>{{Contract__c.Incoterms__c}}</t>
-        </is>
-      </c>
-      <c r="H10" s="5" t="n"/>
-      <c r="I10" s="5" t="n"/>
-      <c r="J10" s="5" t="n"/>
-      <c r="K10" s="5" t="n"/>
-      <c r="L10" s="5" t="n"/>
-      <c r="M10" s="5" t="n"/>
-      <c r="N10" s="4" t="n"/>
+      <c r="D10" s="13" t="n"/>
+      <c r="E10" s="13" t="n"/>
+      <c r="F10" s="7" t="n"/>
+      <c r="G10" s="14" t="inlineStr">
+        <is>
+          <t>FREIGHT: {{#if Contract__c.Incoterms__c 'contains' 'FREIGHT'}}☑{{else}}☐{{/if}}
+PREPAID: {{#if Contract__c.Incoterms__c 'contains' 'PREPAID'}}☑{{else}}☐{{/if}}
+COLLECT: {{#if Contract__c.Incoterms__c 'contains' 'COLLECT'}}☑{{else}}☐{{/if}}</t>
+        </is>
+      </c>
+      <c r="H10" s="8" t="n"/>
+      <c r="I10" s="8" t="n"/>
+      <c r="J10" s="8" t="n"/>
+      <c r="K10" s="8" t="n"/>
+      <c r="L10" s="8" t="n"/>
+      <c r="M10" s="8" t="n"/>
+      <c r="N10" s="8" t="n"/>
     </row>
     <row r="11" ht="25" customHeight="1">
       <c r="A11" s="9" t="n"/>
       <c r="B11" s="10" t="n"/>
-      <c r="C11" s="3" t="inlineStr">
-        <is>
-          <t>PACKING:</t>
-        </is>
-      </c>
-      <c r="D11" s="5" t="n"/>
-      <c r="E11" s="5" t="n"/>
-      <c r="F11" s="4" t="n"/>
-      <c r="G11" s="3" t="inlineStr">
-        <is>
-          <t>SHIPPING SCHEDULE:</t>
-        </is>
-      </c>
-      <c r="H11" s="5" t="n"/>
-      <c r="I11" s="5" t="n"/>
-      <c r="J11" s="5" t="n"/>
-      <c r="K11" s="5" t="n"/>
-      <c r="L11" s="5" t="n"/>
-      <c r="M11" s="5" t="n"/>
-      <c r="N11" s="4" t="n"/>
+      <c r="C11" s="9" t="n"/>
+      <c r="F11" s="10" t="n"/>
+      <c r="G11" s="8" t="n"/>
+      <c r="H11" s="8" t="n"/>
+      <c r="I11" s="8" t="n"/>
+      <c r="J11" s="8" t="n"/>
+      <c r="K11" s="8" t="n"/>
+      <c r="L11" s="8" t="n"/>
+      <c r="M11" s="8" t="n"/>
+      <c r="N11" s="8" t="n"/>
     </row>
     <row r="12" ht="25" customHeight="1">
       <c r="A12" s="9" t="n"/>
       <c r="B12" s="10" t="n"/>
-      <c r="C12" s="6" t="inlineStr">
-        <is>
-          <t>{{Contract__c.Packing__c}}</t>
-        </is>
-      </c>
-      <c r="D12" s="5" t="n"/>
-      <c r="E12" s="5" t="n"/>
-      <c r="F12" s="4" t="n"/>
-      <c r="G12" s="6" t="inlineStr">
-        <is>
-          <t>{{Contract__c.Shipping_Schedule__c}}</t>
-        </is>
-      </c>
-      <c r="H12" s="5" t="n"/>
-      <c r="I12" s="5" t="n"/>
-      <c r="J12" s="5" t="n"/>
-      <c r="K12" s="5" t="n"/>
-      <c r="L12" s="5" t="n"/>
-      <c r="M12" s="5" t="n"/>
-      <c r="N12" s="4" t="n"/>
+      <c r="C12" s="11" t="n"/>
+      <c r="D12" s="15" t="n"/>
+      <c r="E12" s="15" t="n"/>
+      <c r="F12" s="12" t="n"/>
+      <c r="G12" s="8" t="n"/>
+      <c r="H12" s="8" t="n"/>
+      <c r="I12" s="8" t="n"/>
+      <c r="J12" s="8" t="n"/>
+      <c r="K12" s="8" t="n"/>
+      <c r="L12" s="8" t="n"/>
+      <c r="M12" s="8" t="n"/>
+      <c r="N12" s="8" t="n"/>
     </row>
     <row r="13" ht="25" customHeight="1">
       <c r="A13" s="9" t="n"/>
       <c r="B13" s="10" t="n"/>
       <c r="C13" s="3" t="inlineStr">
         <is>
-          <t>TERMS OF SALE:</t>
+          <t>PACKING:</t>
         </is>
       </c>
       <c r="D13" s="5" t="n"/>
@@ -822,7 +815,7 @@
       <c r="F13" s="4" t="n"/>
       <c r="G13" s="3" t="inlineStr">
         <is>
-          <t>TERMS OF PAYMENT:</t>
+          <t>SHIPPING SCHEDULE:</t>
         </is>
       </c>
       <c r="H13" s="5" t="n"/>
@@ -833,58 +826,74 @@
       <c r="M13" s="5" t="n"/>
       <c r="N13" s="4" t="n"/>
     </row>
-    <row r="14" ht="20" customHeight="1">
+    <row r="14" ht="45" customHeight="1">
       <c r="A14" s="9" t="n"/>
       <c r="B14" s="10" t="n"/>
-      <c r="C14" s="13" t="inlineStr">
+      <c r="C14" s="6" t="inlineStr">
+        <is>
+          <t>{{Contract__c.Packing__c}}</t>
+        </is>
+      </c>
+      <c r="D14" s="5" t="n"/>
+      <c r="E14" s="5" t="n"/>
+      <c r="F14" s="4" t="n"/>
+      <c r="G14" s="6" t="inlineStr">
+        <is>
+          <t>{{Contract__c.Shipping_Schedule__c}}</t>
+        </is>
+      </c>
+      <c r="H14" s="5" t="n"/>
+      <c r="I14" s="5" t="n"/>
+      <c r="J14" s="5" t="n"/>
+      <c r="K14" s="5" t="n"/>
+      <c r="L14" s="5" t="n"/>
+      <c r="M14" s="5" t="n"/>
+      <c r="N14" s="4" t="n"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="9" t="n"/>
+      <c r="B15" s="10" t="n"/>
+      <c r="C15" s="3" t="inlineStr">
+        <is>
+          <t>TERMS OF SALE:</t>
+        </is>
+      </c>
+      <c r="D15" s="5" t="n"/>
+      <c r="E15" s="5" t="n"/>
+      <c r="F15" s="4" t="n"/>
+      <c r="G15" s="3" t="inlineStr">
+        <is>
+          <t>TERMS OF PAYMENT:</t>
+        </is>
+      </c>
+      <c r="H15" s="5" t="n"/>
+      <c r="I15" s="5" t="n"/>
+      <c r="J15" s="5" t="n"/>
+      <c r="K15" s="5" t="n"/>
+      <c r="L15" s="5" t="n"/>
+      <c r="M15" s="5" t="n"/>
+      <c r="N15" s="4" t="n"/>
+    </row>
+    <row r="16" ht="20" customHeight="1">
+      <c r="A16" s="9" t="n"/>
+      <c r="B16" s="10" t="n"/>
+      <c r="C16" s="14" t="inlineStr">
         <is>
           <t>FOB : {{#if Contract__c.Terms_of_Sale__c '==' 'FOB'}}☑{{else}}☐{{/if}}
 C&amp;F : {{#if Contract__c.Terms_of_Sale__c '==' 'C&amp;F'}}☑{{else}}☐{{/if}}
 CIF : {{#if Contract__c.Terms_of_Sale__c '==' 'CIF'}}☑{{else}}☐{{/if}}</t>
         </is>
       </c>
-      <c r="D14" s="8" t="n"/>
-      <c r="E14" s="8" t="n"/>
-      <c r="F14" s="8" t="n"/>
-      <c r="G14" s="13" t="inlineStr">
+      <c r="D16" s="8" t="n"/>
+      <c r="E16" s="8" t="n"/>
+      <c r="F16" s="8" t="n"/>
+      <c r="G16" s="14" t="inlineStr">
         <is>
           <t>IRREVOCABLE LETTER OF CREDIT : {{#if Contract__c.Terms_of_Payment__c '==' 'IRREVOCABLE LETTER OF CREDIT'}}☑{{else}}☐{{/if}}
 T/T AT SIGHT DRAFT           : {{#if Contract__c.Terms_of_Payment__c '==' 'T/T AT SIGHT DRAFT'}}☑{{else}}☐{{/if}}
 CASH IN ADVANCE/WIRE TRANSFER: {{#if Contract__c.Terms_of_Payment__c '==' 'CASH IN ADVANCE/WIRE TRANSFER'}}☑{{else}}☐{{/if}}</t>
         </is>
       </c>
-      <c r="H14" s="8" t="n"/>
-      <c r="I14" s="8" t="n"/>
-      <c r="J14" s="8" t="n"/>
-      <c r="K14" s="8" t="n"/>
-      <c r="L14" s="8" t="n"/>
-      <c r="M14" s="8" t="n"/>
-      <c r="N14" s="8" t="n"/>
-    </row>
-    <row r="15" ht="20" customHeight="1">
-      <c r="A15" s="9" t="n"/>
-      <c r="B15" s="10" t="n"/>
-      <c r="C15" s="8" t="n"/>
-      <c r="D15" s="8" t="n"/>
-      <c r="E15" s="8" t="n"/>
-      <c r="F15" s="8" t="n"/>
-      <c r="G15" s="8" t="n"/>
-      <c r="H15" s="8" t="n"/>
-      <c r="I15" s="8" t="n"/>
-      <c r="J15" s="8" t="n"/>
-      <c r="K15" s="8" t="n"/>
-      <c r="L15" s="8" t="n"/>
-      <c r="M15" s="8" t="n"/>
-      <c r="N15" s="8" t="n"/>
-    </row>
-    <row r="16" ht="20" customHeight="1">
-      <c r="A16" s="11" t="n"/>
-      <c r="B16" s="12" t="n"/>
-      <c r="C16" s="8" t="n"/>
-      <c r="D16" s="8" t="n"/>
-      <c r="E16" s="8" t="n"/>
-      <c r="F16" s="8" t="n"/>
-      <c r="G16" s="8" t="n"/>
       <c r="H16" s="8" t="n"/>
       <c r="I16" s="8" t="n"/>
       <c r="J16" s="8" t="n"/>
@@ -893,18 +902,10 @@
       <c r="M16" s="8" t="n"/>
       <c r="N16" s="8" t="n"/>
     </row>
-    <row r="17">
-      <c r="A17" s="14" t="inlineStr">
-        <is>
-          <t>REMARK NUMBER ON DOCUMENTS :</t>
-        </is>
-      </c>
-      <c r="B17" s="8" t="n"/>
-      <c r="C17" s="14" t="inlineStr">
-        <is>
-          <t>BANK DETAIL: A PLUS MINERAL MATERIAL CORPORATION</t>
-        </is>
-      </c>
+    <row r="17" ht="20" customHeight="1">
+      <c r="A17" s="9" t="n"/>
+      <c r="B17" s="10" t="n"/>
+      <c r="C17" s="8" t="n"/>
       <c r="D17" s="8" t="n"/>
       <c r="E17" s="8" t="n"/>
       <c r="F17" s="8" t="n"/>
@@ -917,19 +918,10 @@
       <c r="M17" s="8" t="n"/>
       <c r="N17" s="8" t="n"/>
     </row>
-    <row r="18" ht="40" customHeight="1">
-      <c r="A18" s="6" t="inlineStr">
-        <is>
-          <t>{{Contract__c.REMARK_NUMBER_ON_DOCUMENTS__c}}</t>
-        </is>
-      </c>
-      <c r="B18" s="8" t="n"/>
-      <c r="C18" s="3" t="inlineStr">
-        <is>
-          <t>Account No: 018.137.261.4117 Bank for Foreign Trade of Viet Nam (Vietcombank), Nam Sai Gon branch
-Swift Code: BFTVVNVX018 ; Tel: 84.8.5413.5124 ; Fax: 84.8.5413.5127</t>
-        </is>
-      </c>
+    <row r="18" ht="20" customHeight="1">
+      <c r="A18" s="11" t="n"/>
+      <c r="B18" s="12" t="n"/>
+      <c r="C18" s="8" t="n"/>
       <c r="D18" s="8" t="n"/>
       <c r="E18" s="8" t="n"/>
       <c r="F18" s="8" t="n"/>
@@ -942,262 +934,263 @@
       <c r="M18" s="8" t="n"/>
       <c r="N18" s="8" t="n"/>
     </row>
-    <row r="20">
-      <c r="A20" s="15" t="inlineStr">
+    <row r="19">
+      <c r="A19" s="16" t="inlineStr">
+        <is>
+          <t>REMARK NUMBER ON DOCUMENTS :</t>
+        </is>
+      </c>
+      <c r="B19" s="8" t="n"/>
+      <c r="C19" s="16" t="inlineStr">
+        <is>
+          <t>BANK DETAIL: A PLUS MINERAL MATERIAL CORPORATION</t>
+        </is>
+      </c>
+      <c r="D19" s="8" t="n"/>
+      <c r="E19" s="8" t="n"/>
+      <c r="F19" s="8" t="n"/>
+      <c r="G19" s="8" t="n"/>
+      <c r="H19" s="8" t="n"/>
+      <c r="I19" s="8" t="n"/>
+      <c r="J19" s="8" t="n"/>
+      <c r="K19" s="8" t="n"/>
+      <c r="L19" s="8" t="n"/>
+      <c r="M19" s="8" t="n"/>
+      <c r="N19" s="8" t="n"/>
+    </row>
+    <row r="20" ht="40" customHeight="1">
+      <c r="A20" s="6" t="inlineStr">
+        <is>
+          <t>{{Contract__c.REMARK_NUMBER_ON_DOCUMENTS__c}}</t>
+        </is>
+      </c>
+      <c r="B20" s="8" t="n"/>
+      <c r="C20" s="3" t="inlineStr">
+        <is>
+          <t>Account No: 018.137.261.4117 Bank for Foreign Trade of Viet Nam (Vietcombank), Nam Sai Gon branch
+Swift Code: BFTVVNVX018 ; Tel: 84.8.5413.5124 ; Fax: 84.8.5413.5127</t>
+        </is>
+      </c>
+      <c r="D20" s="8" t="n"/>
+      <c r="E20" s="8" t="n"/>
+      <c r="F20" s="8" t="n"/>
+      <c r="G20" s="8" t="n"/>
+      <c r="H20" s="8" t="n"/>
+      <c r="I20" s="8" t="n"/>
+      <c r="J20" s="8" t="n"/>
+      <c r="K20" s="8" t="n"/>
+      <c r="L20" s="8" t="n"/>
+      <c r="M20" s="8" t="n"/>
+      <c r="N20" s="8" t="n"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="17" t="inlineStr">
         <is>
           <t>ITEM NO.</t>
         </is>
       </c>
-      <c r="B20" s="15" t="inlineStr">
+      <c r="B22" s="17" t="inlineStr">
         <is>
           <t>PRODUCT DESCRIPTION</t>
         </is>
       </c>
-      <c r="C20" s="15" t="inlineStr">
+      <c r="C22" s="17" t="inlineStr">
         <is>
           <t>SIZE (cm)</t>
         </is>
       </c>
-      <c r="D20" s="15" t="n"/>
-      <c r="E20" s="15" t="n"/>
-      <c r="F20" s="15" t="inlineStr">
+      <c r="D22" s="17" t="n"/>
+      <c r="E22" s="17" t="n"/>
+      <c r="F22" s="17" t="inlineStr">
         <is>
           <t>QUANTITY</t>
         </is>
       </c>
-      <c r="G20" s="15" t="n"/>
-      <c r="H20" s="15" t="n"/>
-      <c r="I20" s="15" t="n"/>
-      <c r="J20" s="15" t="n"/>
-      <c r="K20" s="15" t="n"/>
-      <c r="L20" s="15" t="inlineStr">
+      <c r="G22" s="17" t="n"/>
+      <c r="H22" s="17" t="n"/>
+      <c r="I22" s="17" t="n"/>
+      <c r="J22" s="17" t="n"/>
+      <c r="K22" s="17" t="n"/>
+      <c r="L22" s="17" t="inlineStr">
         <is>
           <t>Unit Price (USD)</t>
         </is>
       </c>
-      <c r="M20" s="15" t="inlineStr">
+      <c r="M22" s="17" t="inlineStr">
         <is>
           <t>Total Price (USD)</t>
         </is>
       </c>
-      <c r="N20" s="15" t="inlineStr">
+      <c r="N22" s="17" t="inlineStr">
         <is>
           <t>Packing (pcs/crate)</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="15" t="n"/>
-      <c r="B21" s="15" t="n"/>
-      <c r="C21" s="15" t="inlineStr">
-        <is>
-          <t>L</t>
-        </is>
-      </c>
-      <c r="D21" s="15" t="inlineStr">
-        <is>
-          <t>W</t>
-        </is>
-      </c>
-      <c r="E21" s="15" t="inlineStr">
-        <is>
-          <t>H</t>
-        </is>
-      </c>
-      <c r="F21" s="15" t="inlineStr">
-        <is>
-          <t>PCS</t>
-        </is>
-      </c>
-      <c r="G21" s="15" t="inlineStr">
-        <is>
-          <t>m2</t>
-        </is>
-      </c>
-      <c r="H21" s="15" t="inlineStr">
-        <is>
-          <t>Crates</t>
-        </is>
-      </c>
-      <c r="I21" s="15" t="inlineStr">
-        <is>
-          <t>m3</t>
-        </is>
-      </c>
-      <c r="J21" s="15" t="inlineStr">
-        <is>
-          <t>Tons</t>
-        </is>
-      </c>
-      <c r="K21" s="15" t="inlineStr">
-        <is>
-          <t>Cont.</t>
-        </is>
-      </c>
-      <c r="L21" s="15" t="n"/>
-      <c r="M21" s="15" t="n"/>
-      <c r="N21" s="15" t="n"/>
-    </row>
-    <row r="22" ht="30" customHeight="1">
-      <c r="A22" s="16" t="inlineStr">
-        <is>
-          <t>{{TableStart:ContractProduct2}}{{Line_number_For_print__c}}</t>
-        </is>
-      </c>
-      <c r="B22" s="13" t="inlineStr">
-        <is>
-          <t>{{Product_Discription__c}}</t>
-        </is>
-      </c>
-      <c r="C22" s="16" t="inlineStr">
-        <is>
-          <t>{{L_PI__c}}</t>
-        </is>
-      </c>
-      <c r="D22" s="16" t="inlineStr">
-        <is>
-          <t>{{W_PI__c}}</t>
-        </is>
-      </c>
-      <c r="E22" s="16" t="inlineStr">
-        <is>
-          <t>{{H_PI__c}}</t>
-        </is>
-      </c>
-      <c r="F22" s="16" t="inlineStr">
-        <is>
-          <t>{{PCS_PI__c}}</t>
-        </is>
-      </c>
-      <c r="G22" s="16" t="inlineStr">
-        <is>
-          <t>{{m2__c}}</t>
-        </is>
-      </c>
-      <c r="H22" s="16" t="inlineStr">
-        <is>
-          <t>{{Crates_PI__c}}</t>
-        </is>
-      </c>
-      <c r="I22" s="16" t="inlineStr">
-        <is>
-          <t>{{m3__c}}</t>
-        </is>
-      </c>
-      <c r="J22" s="16" t="inlineStr">
-        <is>
-          <t>{{Tons__c}}</t>
-        </is>
-      </c>
-      <c r="K22" s="16" t="inlineStr">
-        <is>
-          <t>{{Cont__c}}</t>
-        </is>
-      </c>
-      <c r="L22" s="16" t="inlineStr">
-        <is>
-          <t>{{Sales_Price__c}} {{Charge_Unit__c}}</t>
-        </is>
-      </c>
-      <c r="M22" s="16" t="inlineStr">
-        <is>
-          <t>{{Total_Price_USD__c\# #,##0.##}}</t>
-        </is>
-      </c>
-      <c r="N22" s="16" t="inlineStr">
-        <is>
-          <t>{{Packing_PI__c}} {{TableEnd:ContractProduct2}}</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="17" t="n"/>
       <c r="B23" s="17" t="n"/>
-      <c r="C23" s="17" t="n"/>
-      <c r="D23" s="17" t="n"/>
-      <c r="E23" s="17" t="n"/>
-      <c r="F23" s="17" t="n"/>
-      <c r="G23" s="17" t="n"/>
+      <c r="C23" s="17" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="D23" s="17" t="inlineStr">
+        <is>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="E23" s="17" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="F23" s="17" t="inlineStr">
+        <is>
+          <t>PCS</t>
+        </is>
+      </c>
+      <c r="G23" s="17" t="inlineStr">
+        <is>
+          <t>m2</t>
+        </is>
+      </c>
       <c r="H23" s="17" t="inlineStr">
         <is>
-          <t>{{Contract__c.Total_Crates__c}}</t>
+          <t>Crates</t>
         </is>
       </c>
       <c r="I23" s="17" t="inlineStr">
         <is>
-          <t>{{Contract__c.Total_m3__c}}</t>
+          <t>m3</t>
         </is>
       </c>
       <c r="J23" s="17" t="inlineStr">
         <is>
-          <t>{{Contract__c.Total_Tons__c}}</t>
+          <t>Tons</t>
         </is>
       </c>
       <c r="K23" s="17" t="inlineStr">
         <is>
-          <t>{{Contract__c.Total_Conts__c}}</t>
+          <t>Cont.</t>
         </is>
       </c>
       <c r="L23" s="17" t="n"/>
       <c r="M23" s="17" t="n"/>
       <c r="N23" s="17" t="n"/>
     </row>
-    <row r="24">
-      <c r="A24" s="3" t="inlineStr">
+    <row r="24" ht="30" customHeight="1">
+      <c r="A24" s="18" t="inlineStr">
+        <is>
+          <t>{{TableStart:ContractProduct2}}{{Line_number_For_print__c}}</t>
+        </is>
+      </c>
+      <c r="B24" s="14" t="inlineStr">
+        <is>
+          <t>{{Product_Discription__c}}</t>
+        </is>
+      </c>
+      <c r="C24" s="18" t="inlineStr">
+        <is>
+          <t>{{L_PI__c}}</t>
+        </is>
+      </c>
+      <c r="D24" s="18" t="inlineStr">
+        <is>
+          <t>{{W_PI__c}}</t>
+        </is>
+      </c>
+      <c r="E24" s="18" t="inlineStr">
+        <is>
+          <t>{{H_PI__c}}</t>
+        </is>
+      </c>
+      <c r="F24" s="18" t="inlineStr">
+        <is>
+          <t>{{PCS_PI__c}}</t>
+        </is>
+      </c>
+      <c r="G24" s="18" t="inlineStr">
+        <is>
+          <t>{{m2__c}}</t>
+        </is>
+      </c>
+      <c r="H24" s="18" t="inlineStr">
+        <is>
+          <t>{{Crates_PI__c}}</t>
+        </is>
+      </c>
+      <c r="I24" s="18" t="inlineStr">
+        <is>
+          <t>{{m3__c}}</t>
+        </is>
+      </c>
+      <c r="J24" s="18" t="inlineStr">
+        <is>
+          <t>{{Tons__c}}</t>
+        </is>
+      </c>
+      <c r="K24" s="18" t="inlineStr">
+        <is>
+          <t>{{Cont__c}}</t>
+        </is>
+      </c>
+      <c r="L24" s="18" t="inlineStr">
+        <is>
+          <t>{{Sales_Price__c}} {{Charge_Unit__c}}</t>
+        </is>
+      </c>
+      <c r="M24" s="18" t="inlineStr">
+        <is>
+          <t>{{Total_Price_USD__c\# #,##0.##}}</t>
+        </is>
+      </c>
+      <c r="N24" s="18" t="inlineStr">
+        <is>
+          <t>{{Packing_PI__c}} {{TableEnd:ContractProduct2}}</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="19" t="n"/>
+      <c r="B25" s="19" t="n"/>
+      <c r="C25" s="19" t="n"/>
+      <c r="D25" s="19" t="n"/>
+      <c r="E25" s="19" t="n"/>
+      <c r="F25" s="19" t="n"/>
+      <c r="G25" s="19" t="n"/>
+      <c r="H25" s="19" t="inlineStr">
+        <is>
+          <t>{{Contract__c.Total_Crates__c}}</t>
+        </is>
+      </c>
+      <c r="I25" s="19" t="inlineStr">
+        <is>
+          <t>{{Contract__c.Total_m3__c}}</t>
+        </is>
+      </c>
+      <c r="J25" s="19" t="inlineStr">
+        <is>
+          <t>{{Contract__c.Total_Tons__c}}</t>
+        </is>
+      </c>
+      <c r="K25" s="19" t="inlineStr">
+        <is>
+          <t>{{Contract__c.Total_Conts__c}}</t>
+        </is>
+      </c>
+      <c r="L25" s="19" t="n"/>
+      <c r="M25" s="19" t="n"/>
+      <c r="N25" s="19" t="n"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="3" t="inlineStr">
         <is>
           <t>1. All prices quoted herein are US dollars.
 2. Prices quoted herein for merchandise only are valid for 180 days.
 3. Any changes in shipping costs or insurance rates are for account of the buyer.</t>
         </is>
       </c>
-      <c r="B24" s="8" t="n"/>
-      <c r="C24" s="8" t="n"/>
-      <c r="D24" s="8" t="n"/>
-      <c r="E24" s="8" t="n"/>
-      <c r="F24" s="8" t="n"/>
-      <c r="G24" s="8" t="n"/>
-      <c r="H24" s="8" t="n"/>
-      <c r="I24" s="8" t="n"/>
-      <c r="J24" s="8" t="n"/>
-      <c r="K24" s="17" t="inlineStr">
-        <is>
-          <t>SUBTOTAL</t>
-        </is>
-      </c>
-      <c r="L24" s="5" t="n"/>
-      <c r="M24" s="4" t="n"/>
-      <c r="N24" s="17" t="inlineStr">
-        <is>
-          <t>{{Contract__c.Sub_Total_USD__c\# #,##0.##}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="8" t="n"/>
-      <c r="B25" s="8" t="n"/>
-      <c r="C25" s="8" t="n"/>
-      <c r="D25" s="8" t="n"/>
-      <c r="E25" s="8" t="n"/>
-      <c r="F25" s="8" t="n"/>
-      <c r="G25" s="8" t="n"/>
-      <c r="H25" s="8" t="n"/>
-      <c r="I25" s="8" t="n"/>
-      <c r="J25" s="8" t="n"/>
-      <c r="K25" s="17" t="inlineStr">
-        <is>
-          <t>Fumigation</t>
-        </is>
-      </c>
-      <c r="L25" s="5" t="n"/>
-      <c r="M25" s="4" t="n"/>
-      <c r="N25" s="17" t="inlineStr">
-        <is>
-          <t>{{Contract__c.Fumigation__c}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="8" t="n"/>
       <c r="B26" s="8" t="n"/>
       <c r="C26" s="8" t="n"/>
       <c r="D26" s="8" t="n"/>
@@ -1207,16 +1200,16 @@
       <c r="H26" s="8" t="n"/>
       <c r="I26" s="8" t="n"/>
       <c r="J26" s="8" t="n"/>
-      <c r="K26" s="17" t="inlineStr">
-        <is>
-          <t>Deposit ({{Contract__c.Deposit_Percentage__c}} %)</t>
+      <c r="K26" s="19" t="inlineStr">
+        <is>
+          <t>SUBTOTAL</t>
         </is>
       </c>
       <c r="L26" s="5" t="n"/>
       <c r="M26" s="4" t="n"/>
-      <c r="N26" s="17" t="inlineStr">
-        <is>
-          <t>{{Contract__c.Deposit__c\# #,##0.##}}</t>
+      <c r="N26" s="19" t="inlineStr">
+        <is>
+          <t>{{Contract__c.Sub_Total_USD__c\# #,##0.##}}</t>
         </is>
       </c>
     </row>
@@ -1231,16 +1224,16 @@
       <c r="H27" s="8" t="n"/>
       <c r="I27" s="8" t="n"/>
       <c r="J27" s="8" t="n"/>
-      <c r="K27" s="17" t="inlineStr">
-        <is>
-          <t>Surcharge: {{TableStart:PISurcharge}}{{Name}}</t>
+      <c r="K27" s="19" t="inlineStr">
+        <is>
+          <t>Fumigation</t>
         </is>
       </c>
       <c r="L27" s="5" t="n"/>
       <c r="M27" s="4" t="n"/>
-      <c r="N27" s="17" t="inlineStr">
-        <is>
-          <t>{{Surcharge_amount_USD__c\# #,##0.##}}{{TableEnd:PISurcharge}}</t>
+      <c r="N27" s="19" t="inlineStr">
+        <is>
+          <t>{{Contract__c.Fumigation__c}}</t>
         </is>
       </c>
     </row>
@@ -1255,38 +1248,86 @@
       <c r="H28" s="8" t="n"/>
       <c r="I28" s="8" t="n"/>
       <c r="J28" s="8" t="n"/>
-      <c r="K28" s="17" t="inlineStr">
-        <is>
-          <t>TOTAL:</t>
+      <c r="K28" s="19" t="inlineStr">
+        <is>
+          <t>Deposit ({{Contract__c.Deposit_Percentage__c}} %)</t>
         </is>
       </c>
       <c r="L28" s="5" t="n"/>
       <c r="M28" s="4" t="n"/>
-      <c r="N28" s="17" t="inlineStr">
+      <c r="N28" s="19" t="inlineStr">
+        <is>
+          <t>{{Contract__c.Deposit__c\# #,##0.##}}</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="8" t="n"/>
+      <c r="B29" s="8" t="n"/>
+      <c r="C29" s="8" t="n"/>
+      <c r="D29" s="8" t="n"/>
+      <c r="E29" s="8" t="n"/>
+      <c r="F29" s="8" t="n"/>
+      <c r="G29" s="8" t="n"/>
+      <c r="H29" s="8" t="n"/>
+      <c r="I29" s="8" t="n"/>
+      <c r="J29" s="8" t="n"/>
+      <c r="K29" s="19" t="inlineStr">
+        <is>
+          <t>Surcharge: {{TableStart:PISurcharge}}{{Name}}</t>
+        </is>
+      </c>
+      <c r="L29" s="5" t="n"/>
+      <c r="M29" s="4" t="n"/>
+      <c r="N29" s="19" t="inlineStr">
+        <is>
+          <t>{{Surcharge_amount_USD__c\# #,##0.##}}{{TableEnd:PISurcharge}}</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="8" t="n"/>
+      <c r="B30" s="8" t="n"/>
+      <c r="C30" s="8" t="n"/>
+      <c r="D30" s="8" t="n"/>
+      <c r="E30" s="8" t="n"/>
+      <c r="F30" s="8" t="n"/>
+      <c r="G30" s="8" t="n"/>
+      <c r="H30" s="8" t="n"/>
+      <c r="I30" s="8" t="n"/>
+      <c r="J30" s="8" t="n"/>
+      <c r="K30" s="19" t="inlineStr">
+        <is>
+          <t>TOTAL:</t>
+        </is>
+      </c>
+      <c r="L30" s="5" t="n"/>
+      <c r="M30" s="4" t="n"/>
+      <c r="N30" s="19" t="inlineStr">
         <is>
           <t>{{Contract__c.Total_Price_USD__c\# #,##0.##}}</t>
         </is>
       </c>
     </row>
-    <row r="30">
-      <c r="C30" s="18" t="inlineStr">
+    <row r="32">
+      <c r="C32" s="20" t="inlineStr">
         <is>
           <t>FOR AND ON BEHALF OF BUYER</t>
         </is>
       </c>
-      <c r="K30" s="18" t="inlineStr">
+      <c r="K32" s="20" t="inlineStr">
         <is>
           <t>FOR AND ON BEHALF OF SELLER</t>
         </is>
       </c>
     </row>
-    <row r="34">
-      <c r="C34" s="18" t="inlineStr">
+    <row r="36">
+      <c r="C36" s="20" t="inlineStr">
         <is>
           <t>A PLUS CORP</t>
         </is>
       </c>
-      <c r="K34" s="18" t="inlineStr">
+      <c r="K36" s="20" t="inlineStr">
         <is>
           <t>{{Contract__c.Account__r.Name}}</t>
         </is>
@@ -1294,57 +1335,57 @@
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="M20:M21"/>
-    <mergeCell ref="F20:K20"/>
-    <mergeCell ref="G12:N12"/>
-    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="N22:N23"/>
     <mergeCell ref="C8:F8"/>
-    <mergeCell ref="G11:N11"/>
-    <mergeCell ref="A10:B16"/>
+    <mergeCell ref="G16:N18"/>
+    <mergeCell ref="A10:B18"/>
+    <mergeCell ref="C22:E22"/>
     <mergeCell ref="C7:F7"/>
     <mergeCell ref="K7:N7"/>
+    <mergeCell ref="C32:F32"/>
     <mergeCell ref="C13:F13"/>
     <mergeCell ref="K6:N6"/>
+    <mergeCell ref="A26:J30"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="F22:K22"/>
     <mergeCell ref="K27:M27"/>
-    <mergeCell ref="C34:F34"/>
     <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="L20:L21"/>
     <mergeCell ref="A6:B8"/>
-    <mergeCell ref="G10:N10"/>
-    <mergeCell ref="K30:N30"/>
-    <mergeCell ref="K34:N34"/>
+    <mergeCell ref="C15:F15"/>
     <mergeCell ref="G13:N13"/>
     <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C17:N17"/>
-    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="G10:N12"/>
     <mergeCell ref="K5:N5"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="K36:N36"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="A22:A23"/>
     <mergeCell ref="K28:M28"/>
     <mergeCell ref="G8:J8"/>
+    <mergeCell ref="G15:N15"/>
+    <mergeCell ref="C19:N19"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A24:J28"/>
     <mergeCell ref="G7:J7"/>
-    <mergeCell ref="C14:F16"/>
-    <mergeCell ref="C18:N18"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="G14:N14"/>
+    <mergeCell ref="K32:N32"/>
     <mergeCell ref="E3:J3"/>
-    <mergeCell ref="K25:M25"/>
+    <mergeCell ref="K30:M30"/>
+    <mergeCell ref="C10:F12"/>
     <mergeCell ref="G6:J6"/>
     <mergeCell ref="C9:F9"/>
-    <mergeCell ref="K24:M24"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A19:B19"/>
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="G14:N16"/>
-    <mergeCell ref="N20:N21"/>
+    <mergeCell ref="K29:M29"/>
+    <mergeCell ref="C16:F18"/>
     <mergeCell ref="K8:N8"/>
-    <mergeCell ref="C11:F11"/>
     <mergeCell ref="K26:M26"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="G9:N9"/>
     <mergeCell ref="G5:J5"/>
+    <mergeCell ref="C36:F36"/>
+    <mergeCell ref="C20:N20"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>